<commit_message>
Update CORRIDAS TK MULTIMARCAS.xlsx
</commit_message>
<xml_diff>
--- a/CORRIDAS TK MULTIMARCAS.xlsx
+++ b/CORRIDAS TK MULTIMARCAS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Documents\GitHub\CORRIDAS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3C3747D6-FF5F-4A2A-9D86-C5CCFB0F10F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A85D4FEE-C493-4316-B161-3B2D3E2479AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{BA201D9A-D5BA-455E-A537-71F0991FBCDD}"/>
   </bookViews>
@@ -589,8 +589,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5F9604B-4253-4656-9EE1-52445E75917C}">
   <dimension ref="A1:B65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E52" sqref="E52"/>
+    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
+      <selection activeCell="A42" sqref="A42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -815,7 +815,9 @@
       <c r="B29" s="14"/>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="12"/>
+      <c r="A30" s="12">
+        <v>0</v>
+      </c>
       <c r="B30" s="8"/>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
@@ -825,7 +827,9 @@
       <c r="B31" s="14"/>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="12"/>
+      <c r="A32" s="12">
+        <v>0</v>
+      </c>
       <c r="B32" s="8"/>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
@@ -835,7 +839,9 @@
       <c r="B33" s="14"/>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="12"/>
+      <c r="A34" s="12">
+        <v>0</v>
+      </c>
       <c r="B34" s="8"/>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
@@ -845,7 +851,9 @@
       <c r="B35" s="14"/>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="12"/>
+      <c r="A36" s="12">
+        <v>0</v>
+      </c>
       <c r="B36" s="8"/>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
@@ -855,7 +863,9 @@
       <c r="B37" s="14"/>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="12"/>
+      <c r="A38" s="12">
+        <v>0</v>
+      </c>
       <c r="B38" s="8"/>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
@@ -865,7 +875,9 @@
       <c r="B39" s="14"/>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="12"/>
+      <c r="A40" s="12">
+        <v>0</v>
+      </c>
       <c r="B40" s="8"/>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
@@ -875,7 +887,9 @@
       <c r="B41" s="14"/>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" s="12"/>
+      <c r="A42" s="12">
+        <v>0</v>
+      </c>
       <c r="B42" s="8"/>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
@@ -885,7 +899,9 @@
       <c r="B43" s="14"/>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" s="12"/>
+      <c r="A44" s="12">
+        <v>0</v>
+      </c>
       <c r="B44" s="8"/>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
@@ -895,7 +911,9 @@
       <c r="B45" s="16"/>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" s="12"/>
+      <c r="A46" s="12">
+        <v>0</v>
+      </c>
       <c r="B46" s="8"/>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
@@ -905,7 +923,9 @@
       <c r="B47" s="14"/>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" s="12"/>
+      <c r="A48" s="12">
+        <v>0</v>
+      </c>
       <c r="B48" s="8"/>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
@@ -915,7 +935,9 @@
       <c r="B49" s="14"/>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" s="12"/>
+      <c r="A50" s="12">
+        <v>0</v>
+      </c>
       <c r="B50" s="8"/>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
@@ -925,7 +947,9 @@
       <c r="B51" s="14"/>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" s="12"/>
+      <c r="A52" s="12">
+        <v>0</v>
+      </c>
       <c r="B52" s="8"/>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
@@ -935,7 +959,9 @@
       <c r="B53" s="14"/>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" s="12"/>
+      <c r="A54" s="12">
+        <v>0</v>
+      </c>
       <c r="B54" s="8"/>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
@@ -945,7 +971,9 @@
       <c r="B55" s="14"/>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" s="12"/>
+      <c r="A56" s="12">
+        <v>0</v>
+      </c>
       <c r="B56" s="8"/>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
@@ -955,7 +983,9 @@
       <c r="B57" s="14"/>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" s="12"/>
+      <c r="A58" s="12">
+        <v>0</v>
+      </c>
       <c r="B58" s="8"/>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
@@ -965,7 +995,9 @@
       <c r="B59" s="14"/>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60" s="12"/>
+      <c r="A60" s="12">
+        <v>0</v>
+      </c>
       <c r="B60" s="8"/>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
@@ -975,7 +1007,9 @@
       <c r="B61" s="14"/>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62" s="12"/>
+      <c r="A62" s="12">
+        <v>0</v>
+      </c>
       <c r="B62" s="8"/>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
@@ -985,7 +1019,9 @@
       <c r="B63" s="14"/>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A64" s="12"/>
+      <c r="A64" s="12">
+        <v>0</v>
+      </c>
       <c r="B64" s="8"/>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>